<commit_message>
AutoDS OptAnalyser Bug report tronc optimisées dans specs analyses + ajout colonne optim/non optim, via nvelle fonctionnalité colonne neutre traversante + Optimiser/Analyser/Optanalyser Suppression doublons specs avant exécution
</commit_message>
<xml_diff>
--- a/autods/refin/ACDC2019-Naturalist-ExtraitSpecsOptanalyses.xlsx
+++ b/autods/refin/ACDC2019-Naturalist-ExtraitSpecsOptanalyses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eCloud\DistanceSampling\autods\refin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\perso\autods\refin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCC30DD-9CA4-41A0-B345-6F1FAC37EA99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139E11E9-7A1F-49A1-8210-94A6E01A145C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13965" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1944" yWindow="720" windowWidth="28188" windowHeight="14844" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Echant1_impl" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="27">
   <si>
     <t>Passage</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>MultiOpt</t>
+  </si>
+  <si>
+    <t>Duplicate, to check auto-removal</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -468,15 +474,15 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -490,7 +496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -504,7 +510,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -514,6 +520,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -525,15 +532,15 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -547,7 +554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -561,7 +568,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>18</v>
       </c>
@@ -580,13 +587,13 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -594,7 +601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -602,36 +609,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -656,8 +665,11 @@
       <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -671,7 +683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -688,7 +700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -705,7 +717,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -725,7 +737,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -748,7 +760,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -762,7 +774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -779,7 +791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -796,7 +808,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -809,14 +821,14 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10">
-        <v>15</v>
-      </c>
       <c r="F10">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -830,18 +842,15 @@
         <v>18</v>
       </c>
       <c r="E11">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F11">
         <v>300</v>
       </c>
-      <c r="G11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -850,10 +859,19 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>300</v>
+      </c>
+      <c r="G12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -866,11 +884,8 @@
       <c r="D13" t="s">
         <v>17</v>
       </c>
-      <c r="F13">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -884,13 +899,10 @@
         <v>17</v>
       </c>
       <c r="F14">
-        <v>500</v>
-      </c>
-      <c r="G14">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -901,10 +913,16 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>500</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -917,11 +935,8 @@
       <c r="D16" t="s">
         <v>18</v>
       </c>
-      <c r="F16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -935,37 +950,56 @@
         <v>18</v>
       </c>
       <c r="F17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18">
         <v>600</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474A5133-9B74-4D19-823B-523AF343B54A}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -990,8 +1024,11 @@
       <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1005,7 +1042,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1022,7 +1059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1039,7 +1076,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1062,7 +1099,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1076,7 +1113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1093,7 +1130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1110,7 +1147,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1123,37 +1160,59 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E9">
+      <c r="F9">
+        <v>350</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10">
         <v>15</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>370</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B23091B-ECC4-4DEB-9AF9-B2657F5DC316}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1178,8 +1237,11 @@
       <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1202,9 +1264,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1213,61 +1275,64 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
       </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
       <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1276,42 +1341,89 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>200</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
         <v>50</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F9" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H9" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>